<commit_message>
Refactoring to use Util to generate actions
</commit_message>
<xml_diff>
--- a/demos/excel/family.xlsx
+++ b/demos/excel/family.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="17715" windowHeight="17895" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="37140" windowHeight="18570" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
   <si>
     <t>Feature</t>
   </si>
@@ -88,6 +88,48 @@
   </si>
   <si>
     <t>Mother</t>
+  </si>
+  <si>
+    <t>albert</t>
+  </si>
+  <si>
+    <t>paul</t>
+  </si>
+  <si>
+    <t>isa</t>
+  </si>
+  <si>
+    <t>lea</t>
+  </si>
+  <si>
+    <t>elias</t>
+  </si>
+  <si>
+    <t>katell</t>
+  </si>
+  <si>
+    <t>dave</t>
+  </si>
+  <si>
+    <t>clara</t>
+  </si>
+  <si>
+    <t>bryan</t>
+  </si>
+  <si>
+    <t>fiona</t>
+  </si>
+  <si>
+    <t>alain</t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t>Some documentation about Albert
+Multiple lines
+* Item 1
+* Item 2</t>
   </si>
 </sst>
 </file>
@@ -148,7 +190,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -490,18 +534,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="56.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="6" t="s">
         <v>2</v>
       </c>
@@ -520,127 +565,198 @@
       <c r="F1" s="6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
+      <c r="G1" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="90">
+      <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>18</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="D2" s="7">
         <v>17236</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
+      <c r="C3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
+      <c r="C4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E5" t="s">
+      <c r="C5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E6" t="s">
+      <c r="C6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="s">
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" t="s">
+      <c r="C7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E8" t="s">
+      <c r="C8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" t="s">
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E9" t="s">
+      <c r="C9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" t="s">
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E10" t="s">
+      <c r="C10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" t="s">
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E11" t="s">
+      <c r="C11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" t="s">
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E12" t="s">
+      <c r="C12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="G12" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>